<commit_message>
Update to the current progress
</commit_message>
<xml_diff>
--- a/Data/Manufacturing.xlsx
+++ b/Data/Manufacturing.xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjwefGOyachIYZKYjmUr/wVoGThRg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhTYpsSWKXtBRzpCQsQ+On7Rcad8w=="/>
     </ext>
   </extLst>
 </workbook>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -308,6 +308,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -560,10 +566,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.86"/>
-    <col customWidth="1" min="3" max="3" width="25.29"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3726,54 +3729,61 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.14"/>
-    <col customWidth="1" min="2" max="2" width="53.86"/>
-    <col customWidth="1" min="3" max="3" width="51.43"/>
-    <col customWidth="1" min="4" max="4" width="29.71"/>
-    <col customWidth="1" min="5" max="5" width="55.14"/>
-    <col customWidth="1" min="6" max="6" width="39.71"/>
-    <col customWidth="1" min="7" max="7" width="36.0"/>
-    <col customWidth="1" min="8" max="8" width="40.29"/>
-    <col customWidth="1" min="9" max="9" width="16.14"/>
-    <col customWidth="1" min="10" max="10" width="40.0"/>
-    <col customWidth="1" min="11" max="11" width="34.86"/>
-    <col customWidth="1" min="12" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="39.57"/>
+    <col customWidth="1" min="3" max="3" width="33.57"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -29041,9 +29051,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="10" width="8.71"/>
-    <col customWidth="1" min="11" max="11" width="12.43"/>
-    <col customWidth="1" min="12" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>